<commit_message>
Add car data io
</commit_message>
<xml_diff>
--- a/scripts/example_seq2seq.xlsx
+++ b/scripts/example_seq2seq.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>what what do do EOS</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>how let me would into in options for you EOS</t>
+  </si>
+  <si>
+    <t>great let me do the reservation</t>
+  </si>
+  <si>
+    <t>I see. thank you.</t>
   </si>
 </sst>
 </file>
@@ -401,17 +407,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="37" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -481,6 +487,14 @@
         <v>14</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>